<commit_message>
updated test case status and MnS in DiscountReport
</commit_message>
<xml_diff>
--- a/Library/excelResultTestPackBillingReports_MPHV2.1.9A.xlsx
+++ b/Library/excelResultTestPackBillingReports_MPHV2.1.9A.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\QA\AutomationTest\Library\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\QA\Automation\AutomationTest\Library\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="28200" yWindow="0" windowWidth="13905" windowHeight="12300"/>
+    <workbookView xWindow="28200" yWindow="0" windowWidth="13908" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="test" sheetId="1" r:id="rId1"/>
@@ -459,20 +459,20 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="54.5703125" customWidth="1"/>
+    <col min="1" max="1" width="54.5546875" customWidth="1"/>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.7109375" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" customWidth="1"/>
     <col min="6" max="6" width="22" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -495,7 +495,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -514,7 +514,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
@@ -533,7 +533,7 @@
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>13</v>
       </c>
@@ -554,7 +554,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>16</v>
       </c>
@@ -575,7 +575,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>18</v>
       </c>
@@ -594,7 +594,7 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>20</v>
       </c>
@@ -613,8 +613,8 @@
       <c r="F7" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="G7" s="5" t="s">
-        <v>14</v>
+      <c r="G7" s="4" t="s">
+        <v>8</v>
       </c>
       <c r="I7" t="s">
         <v>22</v>

</xml_diff>